<commit_message>
1d2r y 2d2r modificados
</commit_message>
<xml_diff>
--- a/Trabajo_3/Fit_model_1D2R.xlsx
+++ b/Trabajo_3/Fit_model_1D2R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\GGE\Trabajos_GGE\Trabajo_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B709B759-8EF1-4B92-BCD6-9F48994CAF43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABDBDDE-9E63-4663-8489-749F7E0DB320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1944" yWindow="768" windowWidth="16404" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.76600000000000001</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="C2">
         <v>1.0800000000000001E-8</v>

</xml_diff>